<commit_message>
Implementando o CRUD de entidade
</commit_message>
<xml_diff>
--- a/Catálogo de Erros API.xlsx
+++ b/Catálogo de Erros API.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/403cdc586fcb00d5/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Technology\Sistemas\Gabriel\ASPNET\Personal\FinanSist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCF9754A-D975-42D5-BEC0-BA882C2790A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6DC620-256D-4E98-977F-25400CF606E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0448C77B-701D-40CE-B106-8F1EE3774548}"/>
+    <workbookView xWindow="2568" yWindow="2424" windowWidth="17196" windowHeight="9372" xr2:uid="{0448C77B-701D-40CE-B106-8F1EE3774548}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD4EDD3-293F-445D-9D64-BD10B399DF5B}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implementando classe de despesa
</commit_message>
<xml_diff>
--- a/Catálogo de Erros API.xlsx
+++ b/Catálogo de Erros API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Technology\Sistemas\Gabriel\ASPNET\Personal\FinanSist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B65CC49-F6A1-4C18-B0FA-A4B783BF568E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D596EBC-B9EE-4D0F-9A57-FF1CF3EC4EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-192" yWindow="2004" windowWidth="17304" windowHeight="8892" xr2:uid="{0448C77B-701D-40CE-B106-8F1EE3774548}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0448C77B-701D-40CE-B106-8F1EE3774548}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Código</t>
   </si>
@@ -179,6 +179,69 @@
   </si>
   <si>
     <t>Tag/Delete</t>
+  </si>
+  <si>
+    <t>Tag/Get</t>
+  </si>
+  <si>
+    <t>Tag/Pesquisar</t>
+  </si>
+  <si>
+    <t>Despesa/Create</t>
+  </si>
+  <si>
+    <t>Despesa/Update</t>
+  </si>
+  <si>
+    <t>E0026</t>
+  </si>
+  <si>
+    <t>E0027</t>
+  </si>
+  <si>
+    <t>E0028</t>
+  </si>
+  <si>
+    <t>E0029</t>
+  </si>
+  <si>
+    <t>E0030</t>
+  </si>
+  <si>
+    <t>E0031</t>
+  </si>
+  <si>
+    <t>E0032</t>
+  </si>
+  <si>
+    <t>E0033</t>
+  </si>
+  <si>
+    <t>E0034</t>
+  </si>
+  <si>
+    <t>E0035</t>
+  </si>
+  <si>
+    <t>E0036</t>
+  </si>
+  <si>
+    <t>E0037</t>
+  </si>
+  <si>
+    <t>E0038</t>
+  </si>
+  <si>
+    <t>E0039</t>
+  </si>
+  <si>
+    <t>E0040</t>
+  </si>
+  <si>
+    <t>Despesa/Delete</t>
+  </si>
+  <si>
+    <t>Despesa/Get</t>
   </si>
 </sst>
 </file>
@@ -554,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD4EDD3-293F-445D-9D64-BD10B399DF5B}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,20 +808,113 @@
       <c r="A23" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="B24" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="B25" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>